<commit_message>
"Added Logged In Validation"
</commit_message>
<xml_diff>
--- a/testData/zumicData.xlsx
+++ b/testData/zumicData.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="-105" yWindow="-105" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519"/>
   <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
@@ -455,7 +455,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -466,14 +466,14 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="31.7109375" customWidth="1"/>
-    <col min="5" max="5" width="16.42578125" customWidth="1"/>
-    <col min="6" max="6" width="16.140625" customWidth="1"/>
+    <col min="2" max="2" width="34.85546875" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">

</xml_diff>